<commit_message>
2003 Criminal Offenses and Disciplinary Actions refresh
</commit_message>
<xml_diff>
--- a/ope.ed.gov/2003/criminal-offenses-noncampus-virginia-colleges-and-universities-crime-2003.xlsx
+++ b/ope.ed.gov/2003/criminal-offenses-noncampus-virginia-colleges-and-universities-crime-2003.xlsx
@@ -13,16 +13,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
-    <t>Criminal Offenses - Noncampus</t>
-  </si>
-  <si>
-    <t>Survey year</t>
-  </si>
-  <si>
-    <t>Unitid</t>
-  </si>
-  <si>
-    <t>Institution name</t>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>UnitID</t>
+  </si>
+  <si>
+    <t>Institution Name</t>
   </si>
   <si>
     <t>Campus ID</t>
@@ -34,28 +31,28 @@
     <t>Institution Size</t>
   </si>
   <si>
-    <t>Murder/Non-negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Negligent manslaughter</t>
-  </si>
-  <si>
-    <t>Sex offenses - Forcible</t>
-  </si>
-  <si>
-    <t>Sex offenses - Non-forcible</t>
+    <t>Murder/Non-Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Negligent Manslaughter</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Forcible</t>
+  </si>
+  <si>
+    <t>Sex Offenses - Non-Forcible</t>
   </si>
   <si>
     <t>Robbery</t>
   </si>
   <si>
-    <t>Aggravated assault</t>
+    <t>Aggravated Assault</t>
   </si>
   <si>
     <t>Burglary</t>
   </si>
   <si>
-    <t>Motor vehicle theft</t>
+    <t>Motor Vehicle Theft</t>
   </si>
   <si>
     <t>Arson</t>
@@ -409,52 +406,94 @@
       <c t="s" s="1" r="A1">
         <v>0</v>
       </c>
+      <c t="s" s="1" r="B1">
+        <v>1</v>
+      </c>
+      <c t="s" s="1" r="C1">
+        <v>2</v>
+      </c>
+      <c t="s" s="1" r="D1">
+        <v>3</v>
+      </c>
+      <c t="s" s="1" r="E1">
+        <v>4</v>
+      </c>
+      <c t="s" s="1" r="F1">
+        <v>5</v>
+      </c>
+      <c t="s" s="1" r="G1">
+        <v>6</v>
+      </c>
+      <c t="s" s="1" r="H1">
+        <v>7</v>
+      </c>
+      <c t="s" s="1" r="I1">
+        <v>8</v>
+      </c>
+      <c t="s" s="1" r="J1">
+        <v>9</v>
+      </c>
+      <c t="s" s="1" r="K1">
+        <v>10</v>
+      </c>
+      <c t="s" s="1" r="L1">
+        <v>11</v>
+      </c>
+      <c t="s" s="1" r="M1">
+        <v>12</v>
+      </c>
+      <c t="s" s="1" r="N1">
+        <v>13</v>
+      </c>
+      <c t="s" s="1" r="O1">
+        <v>14</v>
+      </c>
     </row>
     <row r="2">
-      <c t="s" s="1" r="A2">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="B2">
-        <v>2</v>
+      <c s="1" r="A2">
+        <v>2003.0</v>
+      </c>
+      <c s="1" r="B2">
+        <v>231554.0</v>
       </c>
       <c t="s" s="1" r="C2">
-        <v>3</v>
-      </c>
-      <c t="s" s="1" r="D2">
-        <v>4</v>
+        <v>15</v>
+      </c>
+      <c s="1" r="D2">
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E2">
-        <v>5</v>
-      </c>
-      <c t="s" s="1" r="F2">
-        <v>6</v>
-      </c>
-      <c t="s" s="1" r="G2">
-        <v>7</v>
-      </c>
-      <c t="s" s="1" r="H2">
-        <v>8</v>
-      </c>
-      <c t="s" s="1" r="I2">
-        <v>9</v>
-      </c>
-      <c t="s" s="1" r="J2">
-        <v>10</v>
-      </c>
-      <c t="s" s="1" r="K2">
-        <v>11</v>
-      </c>
-      <c t="s" s="1" r="L2">
-        <v>12</v>
-      </c>
-      <c t="s" s="1" r="M2">
-        <v>13</v>
-      </c>
-      <c t="s" s="1" r="N2">
-        <v>14</v>
-      </c>
-      <c t="s" s="1" r="O2">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c s="1" r="F2">
+        <v>731.0</v>
+      </c>
+      <c s="1" r="G2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="H2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="I2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="J2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="K2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="L2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="M2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="N2">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="O2">
+        <v>0.0</v>
       </c>
     </row>
     <row r="3">
@@ -462,19 +501,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B3">
-        <v>231554.0</v>
+        <v>231712.0</v>
       </c>
       <c t="s" s="1" r="C3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c s="1" r="D3">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c s="1" r="F3">
-        <v>731.0</v>
+        <v>4812.0</v>
       </c>
       <c s="1" r="G3">
         <v>0.0</v>
@@ -509,19 +548,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B4">
-        <v>231712.0</v>
+        <v>231624.0</v>
       </c>
       <c t="s" s="1" r="C4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c s="1" r="D4">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c s="1" r="F4">
-        <v>4812.0</v>
+        <v>7749.0</v>
       </c>
       <c s="1" r="G4">
         <v>0.0</v>
@@ -556,19 +595,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B5">
-        <v>231624.0</v>
+        <v>231970.0</v>
       </c>
       <c t="s" s="1" r="C5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c s="1" r="D5">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c s="1" r="F5">
-        <v>7749.0</v>
+        <v>638.0</v>
       </c>
       <c s="1" r="G5">
         <v>0.0</v>
@@ -603,19 +642,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B6">
-        <v>231970.0</v>
+        <v>442806.0</v>
       </c>
       <c t="s" s="1" r="C6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c s="1" r="D6">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E6">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c s="1" r="F6">
-        <v>638.0</v>
+        <v>154.0</v>
       </c>
       <c s="1" r="G6">
         <v>0.0</v>
@@ -650,19 +689,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B7">
-        <v>442806.0</v>
+        <v>232089.0</v>
       </c>
       <c t="s" s="1" r="C7">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c s="1" r="D7">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c s="1" r="F7">
-        <v>154.0</v>
+        <v>954.0</v>
       </c>
       <c s="1" r="G7">
         <v>0.0</v>
@@ -697,19 +736,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B8">
-        <v>232089.0</v>
+        <v>232186.0</v>
       </c>
       <c t="s" s="1" r="C8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c s="1" r="D8">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E8">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c s="1" r="F8">
-        <v>954.0</v>
+        <v>28246.0</v>
       </c>
       <c s="1" r="G8">
         <v>0.0</v>
@@ -744,19 +783,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B9">
-        <v>232186.0</v>
+        <v>232256.0</v>
       </c>
       <c t="s" s="1" r="C9">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c s="1" r="D9">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E9">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c s="1" r="F9">
-        <v>28246.0</v>
+        <v>1039.0</v>
       </c>
       <c s="1" r="G9">
         <v>0.0</v>
@@ -791,19 +830,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B10">
-        <v>232256.0</v>
+        <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C10">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c s="1" r="D10">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E10">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c s="1" r="F10">
-        <v>1039.0</v>
+        <v>16203.0</v>
       </c>
       <c s="1" r="G10">
         <v>0.0</v>
@@ -812,7 +851,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I10">
-        <v>0.0</v>
+        <v>18.0</v>
       </c>
       <c s="1" r="J10">
         <v>0.0</v>
@@ -824,7 +863,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M10">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="N10">
         <v>0.0</v>
@@ -841,13 +880,13 @@
         <v>232423.0</v>
       </c>
       <c t="s" s="1" r="C11">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c s="1" r="D11">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E11">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c s="1" r="F11">
         <v>16203.0</v>
@@ -859,7 +898,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I11">
-        <v>18.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="J11">
         <v>0.0</v>
@@ -871,7 +910,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M11">
-        <v>5.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N11">
         <v>0.0</v>
@@ -885,19 +924,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B12">
-        <v>232423.0</v>
+        <v>232566.0</v>
       </c>
       <c t="s" s="1" r="C12">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c s="1" r="D12">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E12">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c s="1" r="F12">
-        <v>16203.0</v>
+        <v>4252.0</v>
       </c>
       <c s="1" r="G12">
         <v>0.0</v>
@@ -932,19 +971,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B13">
-        <v>232566.0</v>
+        <v>232609.0</v>
       </c>
       <c t="s" s="1" r="C13">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c s="1" r="D13">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E13">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c s="1" r="F13">
-        <v>4252.0</v>
+        <v>2009.0</v>
       </c>
       <c s="1" r="G13">
         <v>0.0</v>
@@ -979,19 +1018,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B14">
-        <v>232609.0</v>
+        <v>232706.0</v>
       </c>
       <c t="s" s="1" r="C14">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c s="1" r="D14">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E14">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c s="1" r="F14">
-        <v>2009.0</v>
+        <v>3741.0</v>
       </c>
       <c s="1" r="G14">
         <v>0.0</v>
@@ -1012,7 +1051,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M14">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="N14">
         <v>0.0</v>
@@ -1026,19 +1065,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B15">
-        <v>232706.0</v>
+        <v>232788.0</v>
       </c>
       <c t="s" s="1" r="C15">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c s="1" r="D15">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E15">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c s="1" r="F15">
-        <v>3741.0</v>
+        <v>2875.0</v>
       </c>
       <c s="1" r="G15">
         <v>0.0</v>
@@ -1059,7 +1098,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="M15">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N15">
         <v>0.0</v>
@@ -1073,19 +1112,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B16">
-        <v>232788.0</v>
+        <v>232867.0</v>
       </c>
       <c t="s" s="1" r="C16">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c s="1" r="D16">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E16">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c s="1" r="F16">
-        <v>2875.0</v>
+        <v>4327.0</v>
       </c>
       <c s="1" r="G16">
         <v>0.0</v>
@@ -1120,19 +1159,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B17">
-        <v>232867.0</v>
+        <v>433299.0</v>
       </c>
       <c t="s" s="1" r="C17">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c s="1" r="D17">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E17">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c s="1" r="F17">
-        <v>4327.0</v>
+        <v>52.0</v>
       </c>
       <c s="1" r="G17">
         <v>0.0</v>
@@ -1167,19 +1206,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B18">
-        <v>433299.0</v>
+        <v>233417.0</v>
       </c>
       <c t="s" s="1" r="C18">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c s="1" r="D18">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E18">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c s="1" r="F18">
-        <v>52.0</v>
+        <v>45.0</v>
       </c>
       <c s="1" r="G18">
         <v>0.0</v>
@@ -1214,19 +1253,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B19">
-        <v>233417.0</v>
+        <v>232937.0</v>
       </c>
       <c t="s" s="1" r="C19">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c s="1" r="D19">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E19">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c s="1" r="F19">
-        <v>45.0</v>
+        <v>6846.0</v>
       </c>
       <c s="1" r="G19">
         <v>0.0</v>
@@ -1261,19 +1300,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B20">
-        <v>232937.0</v>
+        <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C20">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c s="1" r="D20">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c s="1" r="F20">
-        <v>6846.0</v>
+        <v>38097.0</v>
       </c>
       <c s="1" r="G20">
         <v>0.0</v>
@@ -1291,7 +1330,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L20">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M20">
         <v>0.0</v>
@@ -1311,13 +1350,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C21">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c s="1" r="D21">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c t="s" s="1" r="E21">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c s="1" r="F21">
         <v>38097.0</v>
@@ -1338,7 +1377,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L21">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M21">
         <v>0.0</v>
@@ -1358,13 +1397,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C22">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c s="1" r="D22">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c t="s" s="1" r="E22">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c s="1" r="F22">
         <v>38097.0</v>
@@ -1405,13 +1444,13 @@
         <v>232946.0</v>
       </c>
       <c t="s" s="1" r="C23">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c s="1" r="D23">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
       <c t="s" s="1" r="E23">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c s="1" r="F23">
         <v>38097.0</v>
@@ -1449,19 +1488,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B24">
-        <v>232946.0</v>
+        <v>232982.0</v>
       </c>
       <c t="s" s="1" r="C24">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c s="1" r="D24">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E24">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c s="1" r="F24">
-        <v>38097.0</v>
+        <v>20802.0</v>
       </c>
       <c s="1" r="G24">
         <v>0.0</v>
@@ -1496,19 +1535,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B25">
-        <v>232982.0</v>
+        <v>233019.0</v>
       </c>
       <c t="s" s="1" r="C25">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c s="1" r="D25">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E25">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c s="1" r="F25">
-        <v>20802.0</v>
+        <v>3492.0</v>
       </c>
       <c s="1" r="G25">
         <v>0.0</v>
@@ -1543,19 +1582,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B26">
-        <v>233019.0</v>
+        <v>233277.0</v>
       </c>
       <c t="s" s="1" r="C26">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c s="1" r="D26">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E26">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c s="1" r="F26">
-        <v>3492.0</v>
+        <v>9219.0</v>
       </c>
       <c s="1" r="G26">
         <v>0.0</v>
@@ -1590,19 +1629,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B27">
-        <v>233277.0</v>
+        <v>437769.0</v>
       </c>
       <c t="s" s="1" r="C27">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c s="1" r="D27">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E27">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c s="1" r="F27">
-        <v>9219.0</v>
+        <v>480.0</v>
       </c>
       <c s="1" r="G27">
         <v>0.0</v>
@@ -1637,19 +1676,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B28">
-        <v>437769.0</v>
+        <v>233408.0</v>
       </c>
       <c t="s" s="1" r="C28">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c s="1" r="D28">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E28">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c s="1" r="F28">
-        <v>480.0</v>
+        <v>154.0</v>
       </c>
       <c s="1" r="G28">
         <v>0.0</v>
@@ -1684,19 +1723,16 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B29">
-        <v>233408.0</v>
+        <v>435213.0</v>
       </c>
       <c t="s" s="1" r="C29">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c s="1" r="D29">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E29">
-        <v>69</v>
-      </c>
-      <c s="1" r="F29">
-        <v>154.0</v>
+        <v>70</v>
       </c>
       <c s="1" r="G29">
         <v>0.0</v>
@@ -1731,16 +1767,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B30">
-        <v>435213.0</v>
+        <v>233499.0</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c s="1" r="D30">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E30">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c s="1" r="F30">
+        <v>475.0</v>
       </c>
       <c s="1" r="G30">
         <v>0.0</v>
@@ -1775,19 +1814,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B31">
-        <v>233499.0</v>
+        <v>233541.0</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c s="1" r="D31">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E31">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c s="1" r="F31">
-        <v>475.0</v>
+        <v>2851.0</v>
       </c>
       <c s="1" r="G31">
         <v>0.0</v>
@@ -1822,19 +1861,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B32">
-        <v>233541.0</v>
+        <v>233639.0</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c s="1" r="D32">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E32">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c s="1" r="F32">
-        <v>2851.0</v>
+        <v>4894.0</v>
       </c>
       <c s="1" r="G32">
         <v>0.0</v>
@@ -1869,19 +1908,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B33">
-        <v>233639.0</v>
+        <v>440341.0</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c s="1" r="D33">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c s="1" r="F33">
-        <v>4894.0</v>
+        <v>852.0</v>
       </c>
       <c s="1" r="G33">
         <v>0.0</v>
@@ -1899,13 +1938,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L33">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M33">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="N33">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c s="1" r="O33">
         <v>0.0</v>
@@ -1916,19 +1955,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B34">
-        <v>440341.0</v>
+        <v>233897.0</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c s="1" r="D34">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E34">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c s="1" r="F34">
-        <v>852.0</v>
+        <v>1703.0</v>
       </c>
       <c s="1" r="G34">
         <v>0.0</v>
@@ -1946,13 +1985,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L34">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M34">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N34">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O34">
         <v>0.0</v>
@@ -1963,19 +2002,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B35">
-        <v>233897.0</v>
+        <v>233754.0</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c s="1" r="D35">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E35">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c s="1" r="F35">
-        <v>1703.0</v>
+        <v>7889.0</v>
       </c>
       <c s="1" r="G35">
         <v>0.0</v>
@@ -2010,19 +2049,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B36">
-        <v>233754.0</v>
+        <v>233772.0</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c s="1" r="D36">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E36">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c s="1" r="F36">
-        <v>7889.0</v>
+        <v>23088.0</v>
       </c>
       <c s="1" r="G36">
         <v>0.0</v>
@@ -2057,19 +2096,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B37">
-        <v>233772.0</v>
+        <v>232681.0</v>
       </c>
       <c t="s" s="1" r="C37">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c s="1" r="D37">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E37">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c s="1" r="F37">
-        <v>23088.0</v>
+        <v>4792.0</v>
       </c>
       <c s="1" r="G37">
         <v>0.0</v>
@@ -2104,19 +2143,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B38">
-        <v>232681.0</v>
+        <v>233374.0</v>
       </c>
       <c t="s" s="1" r="C38">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c s="1" r="D38">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E38">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c s="1" r="F38">
-        <v>4792.0</v>
+        <v>4444.0</v>
       </c>
       <c s="1" r="G38">
         <v>0.0</v>
@@ -2151,19 +2190,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B39">
-        <v>233374.0</v>
+        <v>234076.0</v>
       </c>
       <c t="s" s="1" r="C39">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c s="1" r="D39">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E39">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c s="1" r="F39">
-        <v>4444.0</v>
+        <v>23077.0</v>
       </c>
       <c s="1" r="G39">
         <v>0.0</v>
@@ -2172,7 +2211,7 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I39">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="J39">
         <v>0.0</v>
@@ -2181,10 +2220,10 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L39">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c s="1" r="M39">
-        <v>0.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="N39">
         <v>0.0</v>
@@ -2198,19 +2237,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B40">
-        <v>234076.0</v>
+        <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C40">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c s="1" r="D40">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E40">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c s="1" r="F40">
-        <v>23077.0</v>
+        <v>26631.0</v>
       </c>
       <c s="1" r="G40">
         <v>0.0</v>
@@ -2225,19 +2264,19 @@
         <v>0.0</v>
       </c>
       <c s="1" r="K40">
-        <v>0.0</v>
+        <v>7.0</v>
       </c>
       <c s="1" r="L40">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c s="1" r="M40">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c s="1" r="N40">
-        <v>0.0</v>
+        <v>6.0</v>
       </c>
       <c s="1" r="O40">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="41">
@@ -2248,13 +2287,13 @@
         <v>234030.0</v>
       </c>
       <c t="s" s="1" r="C41">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c s="1" r="D41">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c t="s" s="1" r="E41">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c s="1" r="F41">
         <v>26631.0</v>
@@ -2266,25 +2305,25 @@
         <v>0.0</v>
       </c>
       <c s="1" r="I41">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="J41">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="K41">
+        <v>0.0</v>
+      </c>
+      <c s="1" r="L41">
         <v>2.0</v>
       </c>
-      <c s="1" r="J41">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="K41">
-        <v>7.0</v>
-      </c>
-      <c s="1" r="L41">
-        <v>5.0</v>
-      </c>
       <c s="1" r="M41">
-        <v>4.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="N41">
-        <v>6.0</v>
+        <v>2.0</v>
       </c>
       <c s="1" r="O41">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="42">
@@ -2292,19 +2331,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B42">
-        <v>234030.0</v>
+        <v>233912.0</v>
       </c>
       <c t="s" s="1" r="C42">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c s="1" r="D42">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c t="s" s="1" r="E42">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c s="1" r="F42">
-        <v>26631.0</v>
+        <v>1124.0</v>
       </c>
       <c s="1" r="G42">
         <v>0.0</v>
@@ -2322,13 +2361,13 @@
         <v>0.0</v>
       </c>
       <c s="1" r="L42">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="M42">
         <v>0.0</v>
       </c>
       <c s="1" r="N42">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
       <c s="1" r="O42">
         <v>0.0</v>
@@ -2339,19 +2378,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B43">
-        <v>233912.0</v>
+        <v>234085.0</v>
       </c>
       <c t="s" s="1" r="C43">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c s="1" r="D43">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E43">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c s="1" r="F43">
-        <v>1124.0</v>
+        <v>1333.0</v>
       </c>
       <c s="1" r="G43">
         <v>0.0</v>
@@ -2386,19 +2425,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B44">
-        <v>234085.0</v>
+        <v>233921.0</v>
       </c>
       <c t="s" s="1" r="C44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c s="1" r="D44">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E44">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c s="1" r="F44">
-        <v>1333.0</v>
+        <v>27755.0</v>
       </c>
       <c s="1" r="G44">
         <v>0.0</v>
@@ -2433,19 +2472,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B45">
-        <v>233921.0</v>
+        <v>234155.0</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c s="1" r="D45">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E45">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c s="1" r="F45">
-        <v>27755.0</v>
+        <v>4933.0</v>
       </c>
       <c s="1" r="G45">
         <v>0.0</v>
@@ -2480,19 +2519,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B46">
-        <v>234155.0</v>
+        <v>233949.0</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c s="1" r="D46">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E46">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c s="1" r="F46">
-        <v>4933.0</v>
+        <v>8124.0</v>
       </c>
       <c s="1" r="G46">
         <v>0.0</v>
@@ -2527,19 +2566,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B47">
-        <v>233949.0</v>
+        <v>234207.0</v>
       </c>
       <c t="s" s="1" r="C47">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c s="1" r="D47">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E47">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c s="1" r="F47">
-        <v>8124.0</v>
+        <v>2137.0</v>
       </c>
       <c s="1" r="G47">
         <v>0.0</v>
@@ -2574,19 +2613,19 @@
         <v>2003.0</v>
       </c>
       <c s="1" r="B48">
-        <v>234207.0</v>
+        <v>234377.0</v>
       </c>
       <c t="s" s="1" r="C48">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c s="1" r="D48">
         <v>1.0</v>
       </c>
       <c t="s" s="1" r="E48">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c s="1" r="F48">
-        <v>2137.0</v>
+        <v>2948.0</v>
       </c>
       <c s="1" r="G48">
         <v>0.0</v>
@@ -2613,53 +2652,6 @@
         <v>0.0</v>
       </c>
       <c s="1" r="O48">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c s="1" r="A49">
-        <v>2003.0</v>
-      </c>
-      <c s="1" r="B49">
-        <v>234377.0</v>
-      </c>
-      <c t="s" s="1" r="C49">
-        <v>108</v>
-      </c>
-      <c s="1" r="D49">
-        <v>1.0</v>
-      </c>
-      <c t="s" s="1" r="E49">
-        <v>109</v>
-      </c>
-      <c s="1" r="F49">
-        <v>2948.0</v>
-      </c>
-      <c s="1" r="G49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="H49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="I49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="J49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="K49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="L49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="M49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="N49">
-        <v>0.0</v>
-      </c>
-      <c s="1" r="O49">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>